<commit_message>
added open account test and extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauri.bhale\IdeaProjects\DataDrivenFW\DataDrienFW\src\test\resources\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A783073-1750-4FCE-93C8-2B095092223B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7755"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="Test_suite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>firstName</t>
   </si>
@@ -37,16 +43,71 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Raman Aruna</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Arora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohit </t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>Gautam</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,14 +133,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -126,7 +198,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -158,9 +230,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -192,6 +282,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -367,19 +475,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,8 +500,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -405,6 +516,60 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>431005</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>431005</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>431005</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -413,25 +578,83 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>